<commit_message>
fixup of many hard coded parameters
</commit_message>
<xml_diff>
--- a/Testing/sample-accounting-transfer.xlsx
+++ b/Testing/sample-accounting-transfer.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3385" uniqueCount="253">
   <si>
     <t>Date</t>
   </si>
@@ -771,6 +771,9 @@
   </si>
   <si>
     <t>FPL</t>
+  </si>
+  <si>
+    <t>2035 Library Rd</t>
   </si>
 </sst>
 </file>
@@ -856,7 +859,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,6 +874,14 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -890,14 +901,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F1:AJ412"/>
+  <dimension ref="F1:AJ414"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G400" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A400" activeCellId="0" sqref="A400"/>
-      <selection pane="bottomRight" activeCell="H412" activeCellId="0" sqref="H412"/>
+      <selection pane="bottomRight" activeCell="G413" activeCellId="0" sqref="413:414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14369,6 +14380,73 @@
         <v>251</v>
       </c>
     </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F413" s="2" t="n">
+        <v>42215</v>
+      </c>
+      <c r="H413" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="L413" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="P413" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="T413" s="0" t="n">
+        <v>44236</v>
+      </c>
+      <c r="V413" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z413" s="4" t="n">
+        <v>23529000445172</v>
+      </c>
+      <c r="AD413" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH413" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AJ413" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F414" s="2" t="n">
+        <v>42215</v>
+      </c>
+      <c r="H414" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="L414" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="P414" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="T414" s="0" t="n">
+        <v>44240</v>
+      </c>
+      <c r="V414" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y414" s="5"/>
+      <c r="Z414" s="4" t="n">
+        <v>23529001000463</v>
+      </c>
+      <c r="AA414" s="4"/>
+      <c r="AB414" s="4"/>
+      <c r="AD414" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH414" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ414" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>